<commit_message>
finishing up code on the QUTO allelic representation
</commit_message>
<xml_diff>
--- a/Analyses/Results/Clustering/STRUCTURE/QUTO_wild_STRUCTURE/QUTO_wild_deltaK.xlsx
+++ b/Analyses/Results/Clustering/STRUCTURE/QUTO_wild_STRUCTURE/QUTO_wild_deltaK.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eschumacher\Documents\GitHub\Ten_Oaks\Analyses\Results\Clustering\STRUCTURE\QUTO_wild_STRUCTURE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34A79C7-AEDA-4E4A-AB67-52A66773F234}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9762EDA4-FD79-404F-B127-CF77AB0D827E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19050" windowHeight="10665" activeTab="4" xr2:uid="{B8FF9A77-FB0D-40F7-BFB4-BCFE592F1F86}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19050" windowHeight="10665" activeTab="3" xr2:uid="{B8FF9A77-FB0D-40F7-BFB4-BCFE592F1F86}"/>
   </bookViews>
   <sheets>
     <sheet name="deltaK" sheetId="1" r:id="rId1"/>
@@ -18971,16 +18971,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>252412</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -19012,16 +19012,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>509587</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>414337</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -24132,7 +24132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6F271F-4929-4C9A-9CF3-E7613791AE93}">
   <dimension ref="A1:F151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
@@ -26891,7 +26891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C42C21C-AD22-4418-91FC-67A49F0217CC}">
   <dimension ref="A1:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>

</xml_diff>